<commit_message>
Added writer_filter_list() to autofilter example.
</commit_message>
<xml_diff>
--- a/test/perl_output/autofilter.xlsx
+++ b/test/perl_output/autofilter.xlsx
@@ -13,6 +13,7 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$51</definedName>
@@ -21,13 +22,14 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet4!$A$1:$D$51</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet5!$A$1:$D$51</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sheet6!$A$1:$D$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Sheet7!$A$1:$D$51</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="24">
   <si>
     <t>Region</t>
   </si>
@@ -3415,7 +3417,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3429,7 +3431,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3443,7 +3445,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3457,7 +3459,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3486,6 +3488,9 @@
       </c>
     </row>
     <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
@@ -3496,7 +3501,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -3538,7 +3543,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -3566,7 +3571,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -3580,7 +3585,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -3594,7 +3599,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -3622,7 +3627,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -3636,7 +3641,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -3664,7 +3669,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -3678,7 +3683,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -3692,7 +3697,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -3706,7 +3711,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -3720,7 +3725,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" hidden="1">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -3734,7 +3739,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:4" hidden="1">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -3748,7 +3753,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -3762,7 +3767,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -3790,7 +3795,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -3818,7 +3823,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:4" hidden="1">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -3832,7 +3837,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -3846,7 +3851,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:4" hidden="1">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -3860,7 +3865,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -3874,7 +3879,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -3888,7 +3893,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:4" hidden="1">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -3902,7 +3907,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:4" hidden="1">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -3930,7 +3935,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:4" hidden="1">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -3944,7 +3949,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:4" hidden="1">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -3958,7 +3963,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:4" hidden="1">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -3972,7 +3977,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:4" hidden="1">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -4000,7 +4005,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:4" hidden="1">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -4014,7 +4019,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:4" hidden="1">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -4028,7 +4033,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:4" hidden="1">
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -4042,7 +4047,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:4" hidden="1">
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -4056,7 +4061,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:4" hidden="1">
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>4</v>
       </c>
@@ -4070,7 +4075,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:4" hidden="1">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -4084,7 +4089,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:4" hidden="1">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -4098,7 +4103,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:4" hidden="1">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -4115,7 +4120,11 @@
   </sheetData>
   <autoFilter ref="A1:D51">
     <filterColumn colId="0">
-      <filters blank="1"/>
+      <filters>
+        <filter val="East"/>
+        <filter val="North"/>
+        <filter val="South"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4148,6 +4157,739 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" hidden="1">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>9000</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" hidden="1">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>5000</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" hidden="1">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>9000</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" hidden="1">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>2000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" hidden="1">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>9000</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>7000</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" hidden="1">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>9000</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" hidden="1">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>1000</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" hidden="1">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>1000</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" hidden="1">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>10000</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" hidden="1">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>6000</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" hidden="1">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>3000</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" hidden="1">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>3000</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" hidden="1">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>7000</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" hidden="1">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>1000</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" hidden="1">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <v>8000</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" hidden="1">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>10000</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" hidden="1">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>7000</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" hidden="1">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>2000</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" hidden="1">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21">
+        <v>7000</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" hidden="1">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22">
+        <v>6000</v>
+      </c>
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" hidden="1">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23">
+        <v>8000</v>
+      </c>
+      <c r="D23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" hidden="1">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>7000</v>
+      </c>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" hidden="1">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>7000</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" hidden="1">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>6000</v>
+      </c>
+      <c r="D26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" hidden="1">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27">
+        <v>8000</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" hidden="1">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>3000</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" hidden="1">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>10000</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" hidden="1">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30">
+        <v>4000</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" hidden="1">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>5000</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" hidden="1">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>1000</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" hidden="1">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>4000</v>
+      </c>
+      <c r="D33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" hidden="1">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34">
+        <v>5000</v>
+      </c>
+      <c r="D34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" hidden="1">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <v>1000</v>
+      </c>
+      <c r="D35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" hidden="1">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36">
+        <v>10000</v>
+      </c>
+      <c r="D36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" hidden="1">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37">
+        <v>7000</v>
+      </c>
+      <c r="D37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" hidden="1">
+      <c r="A38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38">
+        <v>1000</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" hidden="1">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39">
+        <v>10000</v>
+      </c>
+      <c r="D39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" hidden="1">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40">
+        <v>8000</v>
+      </c>
+      <c r="D40" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" hidden="1">
+      <c r="A41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <v>4000</v>
+      </c>
+      <c r="D41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" hidden="1">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <v>5000</v>
+      </c>
+      <c r="D42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" hidden="1">
+      <c r="A43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <v>4000</v>
+      </c>
+      <c r="D43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" hidden="1">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <v>5000</v>
+      </c>
+      <c r="D44" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" hidden="1">
+      <c r="A45" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45">
+        <v>3000</v>
+      </c>
+      <c r="D45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" hidden="1">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46">
+        <v>9000</v>
+      </c>
+      <c r="D46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" hidden="1">
+      <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47">
+        <v>8000</v>
+      </c>
+      <c r="D47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" hidden="1">
+      <c r="A48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48">
+        <v>10000</v>
+      </c>
+      <c r="D48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" hidden="1">
+      <c r="A49" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49">
+        <v>1000</v>
+      </c>
+      <c r="D49" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" hidden="1">
+      <c r="A50" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50">
+        <v>10000</v>
+      </c>
+      <c r="D50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" hidden="1">
+      <c r="A51" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51">
+        <v>6000</v>
+      </c>
+      <c r="D51" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D51">
+    <filterColumn colId="0">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="4" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="20" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>

</xml_diff>